<commit_message>
final commit on 4th OCT. 2018
</commit_message>
<xml_diff>
--- a/dist/assets/studentlist_format.xlsx
+++ b/dist/assets/studentlist_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">userId</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-19_ODD</t>
   </si>
 </sst>
 </file>
@@ -169,15 +172,15 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -211,12 +214,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>